<commit_message>
added metadata for baseline sampling
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianasnowhuffmyer/MyProjects/E5/apulchra_metabolism/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D88D82-302B-7B41-AD8E-DB2F2A44D519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7CD945-ADA0-CF4F-B7A9-4DF5EBF9603A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="1780" windowWidth="21000" windowHeight="14320" activeTab="1" xr2:uid="{368D60C7-8B7D-924B-9BC3-F169020976FA}"/>
+    <workbookView xWindow="6360" yWindow="1780" windowWidth="21000" windowHeight="14320" xr2:uid="{368D60C7-8B7D-924B-9BC3-F169020976FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Initials</t>
   </si>
@@ -71,6 +71,18 @@
   </si>
   <si>
     <t xml:space="preserve">Initial cleaning at start of experiment </t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No mortality observed, tanks running well </t>
+  </si>
+  <si>
+    <t xml:space="preserve">completed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Removed algae from a couple frags, no mortality observed </t>
   </si>
 </sst>
 </file>
@@ -422,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC17A8C-3D5B-A541-B80F-453EF69C9230}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -451,6 +463,40 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>20220929</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>20220930</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -460,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{002E4EA5-7B12-FB44-A21E-50A18B159260}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added daily measurements and airbrushing data
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianasnowhuffmyer/MyProjects/E5/apulchra_metabolism/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA725735-01F7-F84C-AD95-2BBDA534455E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663F66E1-531B-324F-8A77-4A7AB3F83625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="1780" windowWidth="21000" windowHeight="14320" activeTab="1" xr2:uid="{368D60C7-8B7D-924B-9BC3-F169020976FA}"/>
+    <workbookView xWindow="6360" yWindow="1780" windowWidth="21000" windowHeight="14320" xr2:uid="{368D60C7-8B7D-924B-9BC3-F169020976FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
   <si>
     <t>Initials</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Rearranged tanks within table today</t>
+  </si>
+  <si>
+    <t>Rusing on paper clips, will need to replace soon</t>
   </si>
 </sst>
 </file>
@@ -449,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC17A8C-3D5B-A541-B80F-453EF69C9230}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,6 +560,23 @@
         <v>19</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>20221004</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -566,7 +586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{002E4EA5-7B12-FB44-A21E-50A18B159260}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added protein and cell density files, analyzed baseline phys
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianasnowhuffmyer/MyProjects/E5/apulchra_metabolism/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65766C5D-797B-5740-B365-C03EF068E2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBE28C3-1C81-C243-83B4-249C792EF217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6360" yWindow="1780" windowWidth="21000" windowHeight="14320" xr2:uid="{368D60C7-8B7D-924B-9BC3-F169020976FA}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="27">
   <si>
     <t>Initials</t>
   </si>
@@ -467,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC17A8C-3D5B-A541-B80F-453EF69C9230}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -727,6 +727,20 @@
         <v>12</v>
       </c>
       <c r="D16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>20221014</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added logger figures, ran new daily measurements
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianasnowhuffmyer/MyProjects/E5/apulchra_metabolism/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBE28C3-1C81-C243-83B4-249C792EF217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1020B651-B24E-6C42-8533-9D7B4DD75D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6360" yWindow="1780" windowWidth="21000" windowHeight="14320" xr2:uid="{368D60C7-8B7D-924B-9BC3-F169020976FA}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="27">
   <si>
     <t>Initials</t>
   </si>
@@ -467,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC17A8C-3D5B-A541-B80F-453EF69C9230}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -741,6 +741,20 @@
         <v>12</v>
       </c>
       <c r="D17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>20221015</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>